<commit_message>
added arguments to separateFile.C
</commit_message>
<xml_diff>
--- a/filesInfo.xlsx
+++ b/filesInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maral87-local/Desktop/Maral/Projects/Workflow-Presentations/HGCal/Daily/git_HGCal_CE-H_Plates_QA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB13AAA-3106-FF4C-8D08-A7DC313ECB5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2FA5410-098C-0141-972B-7C473B4D2F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5020" yWindow="780" windowWidth="20200" windowHeight="14100" activeTab="1" xr2:uid="{5182EF2D-127D-AE4E-8BE6-3390D8389ED2}"/>
+    <workbookView xWindow="5020" yWindow="780" windowWidth="20200" windowHeight="14100" xr2:uid="{5182EF2D-127D-AE4E-8BE6-3390D8389ED2}"/>
   </bookViews>
   <sheets>
     <sheet name="filesNames" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,6 @@
     <t>allTop_7B_config1_sorted</t>
   </si>
   <si>
-    <t>allBottom_7B_config1_sorted.csv</t>
-  </si>
-  <si>
     <t>CE-H7B-BOTTOM-OUT-03152023_1</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>bottom side features measured</t>
+  </si>
+  <si>
+    <t>allBottom_7B_config1_sorted</t>
   </si>
 </sst>
 </file>
@@ -459,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FABE81-8FA3-8F45-8747-223E0C5289A6}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -472,37 +472,37 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -514,7 +514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA9BA2B5-34DD-D241-81B9-5AB1FBDF5807}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -526,10 +526,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>